<commit_message>
change UI for NhapKho
</commit_message>
<xml_diff>
--- a/DanhSachSanPham.xlsx
+++ b/DanhSachSanPham.xlsx
@@ -148,13 +148,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>7000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>2000.0</v>
+        <v>22000.0</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>11</v>

</xml_diff>